<commit_message>
v0.24 - Operation Complete
</commit_message>
<xml_diff>
--- a/static/paper/CO04_paper.xlsx
+++ b/static/paper/CO04_paper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SnowBall\static\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE646699-E456-4450-99A3-5CF35C77AAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD31871-4B03-4915-A95A-A182D0C5DEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5E3EE22-C542-4402-8654-7D4EE4676255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5E3EE22-C542-4402-8654-7D4EE4676255}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Table" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Prior year control testing documentation rolled forward for reference purposes.</t>
   </si>
@@ -143,23 +143,27 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>오류 조치 여부</t>
+    <r>
+      <t xml:space="preserve">Backup </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>모니터링</t>
+    </r>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>조치 완료 일자</t>
+    <t>모니터링 일자</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>조치여부</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Backup</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Backup 오류 일자</t>
+    <t>승인 일자</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -268,14 +272,14 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="맑은 고딕"/>
-      <family val="3"/>
+      <family val="1"/>
       <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -322,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -557,19 +561,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -603,7 +594,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -680,10 +671,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -700,11 +687,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1360,471 +1343,334 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J31"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="1.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="2"/>
-    <col min="12" max="12" width="9.140625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="2"/>
+    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="2:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="2:8" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="35"/>
-    </row>
-    <row r="4" spans="2:10" s="6" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="2:8" s="6" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="29" t="s">
+      <c r="C4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="D4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="E4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10" t="str">
-        <f>IF(F5="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="12">
         <v>2</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="16" t="str">
-        <f>IF(F6="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="12">
         <v>3</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="16" t="str">
-        <f t="shared" ref="G7:G28" si="0">IF(F7="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="12">
         <v>4</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="12">
         <v>5</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="12">
         <v>6</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="12">
         <v>7</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="12">
         <v>8</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="12">
         <v>9</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="12">
         <v>10</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="12">
         <v>11</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="12">
         <v>12</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="12">
         <v>13</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="12">
         <v>14</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="12">
         <v>15</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="12">
         <v>16</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="12">
         <v>17</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="17"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="12">
         <v>18</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="12">
         <v>19</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
-    </row>
-    <row r="24" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="12">
         <v>20</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
-    </row>
-    <row r="25" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="12">
         <v>21</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17"/>
-    </row>
-    <row r="26" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="12">
         <v>22</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="12">
         <v>23</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="12">
         <v>24</v>
       </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>X</v>
-      </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="18">
         <v>25</v>
       </c>
       <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21" t="str">
-        <f>IF(F29="", "X", "O")</f>
-        <v>X</v>
-      </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-    </row>
-    <row r="30" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:9" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="23" t="s">
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="E31" s="25"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>